<commit_message>
update semester project and assignment 4
</commit_message>
<xml_diff>
--- a/SemesterProject/SemesterProject.xlsx
+++ b/SemesterProject/SemesterProject.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brent\Projects\COMPE361\SemesterProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2684503F-A165-4F40-8DDD-9DEC311E5557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F426AFF1-88FA-44D0-B905-D6792FB83D18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3444" yWindow="936" windowWidth="17280" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>osmanthus</t>
+  </si>
+  <si>
+    <t>admin</t>
   </si>
 </sst>
 </file>
@@ -436,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -466,10 +469,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -477,10 +480,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -488,10 +491,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -499,10 +502,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -510,10 +513,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -521,10 +524,10 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -532,10 +535,10 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -543,9 +546,20 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>